<commit_message>
Filtro provider modal excel
</commit_message>
<xml_diff>
--- a/src/assets/modelo_producto_crear.xlsx
+++ b/src/assets/modelo_producto_crear.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krouz\Desktop\p\pos\poscloud-system\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB40D750-7E6C-46D6-AA82-A1FB52E42AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90779C2-4641-4CAC-83E3-A892FB3F0DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EA0E453A-7D54-47A7-899B-47EA39284D48}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -454,7 +454,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
code provider - loading create excel
</commit_message>
<xml_diff>
--- a/src/assets/modelo_producto_crear.xlsx
+++ b/src/assets/modelo_producto_crear.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krouz\Desktop\p\pos\poscloud-system\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90779C2-4641-4CAC-83E3-A892FB3F0DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD94A0D-0582-4990-8CD3-58B0E4891DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EA0E453A-7D54-47A7-899B-47EA39284D48}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,9 +33,6 @@
     <t>codigo_de_barra</t>
   </si>
   <si>
-    <t>codigo_de_provedor</t>
-  </si>
-  <si>
     <t>precio_base</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t xml:space="preserve">El proveedor tiene que existir </t>
+  </si>
+  <si>
+    <t>codigo_de_proveedor</t>
   </si>
 </sst>
 </file>
@@ -454,7 +454,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,56 +477,56 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
       <c r="P1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="E2" s="3"/>
       <c r="O2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>